<commit_message>
Table corrections: Property and distribution
</commit_message>
<xml_diff>
--- a/final_outputs/figure_b_distribution.xlsx
+++ b/final_outputs/figure_b_distribution.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\international-tax-competitiveness-index\final_outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7556637-7720-4F8C-8C6A-16F3A3F707C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77CFD432-AF46-4B52-9D6E-2F8EF960BA97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{7939B179-B2E8-475D-84F7-774A10E48CF3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Estonia</t>
   </si>
@@ -150,6 +150,12 @@
   </si>
   <si>
     <t>France</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>score</t>
   </si>
 </sst>
 </file>
@@ -165,15 +171,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -181,12 +193,45 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -240,17 +285,17 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$1:$A$38</c:f>
+              <c:f>Sheet1!$A$2:$A$39</c:f>
               <c:strCache>
                 <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>Estonia</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>Latvia</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>New Zealand</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Latvia</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Switzerland</c:v>
@@ -262,25 +307,25 @@
                   <c:v>Luxembourg</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>Turkey</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>Israel</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>Lithuania</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
+                  <c:v>Australia</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>Hungary</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>Turkey</c:v>
-                </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>Slovak Republic</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>Sweden</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Australia</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>Netherlands</c:v>
@@ -289,13 +334,13 @@
                   <c:v>Canada</c:v>
                 </c:pt>
                 <c:pt idx="15">
+                  <c:v>Slovenia</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Norway</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>Germany</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>Slovenia</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Norway</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>Finland</c:v>
@@ -343,26 +388,26 @@
                   <c:v>Poland</c:v>
                 </c:pt>
                 <c:pt idx="33">
+                  <c:v>Portugal</c:v>
+                </c:pt>
+                <c:pt idx="34">
                   <c:v>Chile</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="35">
+                  <c:v>France</c:v>
+                </c:pt>
+                <c:pt idx="36">
                   <c:v>Italy</c:v>
                 </c:pt>
-                <c:pt idx="35">
-                  <c:v>Portugal</c:v>
-                </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="37">
                   <c:v>Colombia</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>France</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$B$38</c:f>
+              <c:f>Sheet1!$B$2:$B$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="38"/>
@@ -370,115 +415,115 @@
                   <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>89.8</c:v>
+                  <c:v>88.5135341952262</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>88.9</c:v>
+                  <c:v>86.134241189157194</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>85.1</c:v>
+                  <c:v>84.690652481164705</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>81.599999999999994</c:v>
+                  <c:v>81.239916001175104</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>80.5</c:v>
+                  <c:v>78.881582113664507</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>78.8</c:v>
+                  <c:v>78.608399513280105</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>77</c:v>
+                  <c:v>78.337865366481296</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>75.5</c:v>
+                  <c:v>76.594188906568206</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>75.3</c:v>
+                  <c:v>75.900087249756496</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>74.8</c:v>
+                  <c:v>75.035801179744695</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>73.7</c:v>
+                  <c:v>74.306844394688696</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>72.400000000000006</c:v>
+                  <c:v>73.265004830263507</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>71.099999999999994</c:v>
+                  <c:v>70.645110016851703</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>70.3</c:v>
+                  <c:v>69.806090563549802</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>68.3</c:v>
+                  <c:v>66.644575644135401</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>67.400000000000006</c:v>
+                  <c:v>66.618664278738095</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>67.099999999999994</c:v>
+                  <c:v>66.613837247704495</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>67</c:v>
+                  <c:v>66.532237268287801</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>66.099999999999994</c:v>
+                  <c:v>65.336679742935203</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>65.5</c:v>
+                  <c:v>65.003846152919294</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>65.3</c:v>
+                  <c:v>64.801428454145807</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>63.6</c:v>
+                  <c:v>61.6265690222736</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>63.3</c:v>
+                  <c:v>61.542648357063399</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>62</c:v>
+                  <c:v>61.4364336931311</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>60.7</c:v>
+                  <c:v>60.115211295109603</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>60.5</c:v>
+                  <c:v>59.952486808300399</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>59.4</c:v>
+                  <c:v>58.878704972371096</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>59.1</c:v>
+                  <c:v>58.520696901632299</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>56.7</c:v>
+                  <c:v>56.090824829985102</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>56.3</c:v>
+                  <c:v>55.7629065934916</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>56.3</c:v>
+                  <c:v>55.483189232205802</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>55.9</c:v>
+                  <c:v>55.298195147353297</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>51.1</c:v>
+                  <c:v>52.075590082840698</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>49.2</c:v>
+                  <c:v>50.4668505874427</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>49</c:v>
+                  <c:v>49.149218022731802</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>47</c:v>
+                  <c:v>48.353582459841199</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>46.1</c:v>
+                  <c:v>46.375963179193903</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -527,7 +572,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -1209,16 +1254,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>121443</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>78581</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>257899</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>35925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>107156</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>50730</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>64500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1543,316 +1588,324 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A3FE8D0-0C40-4651-B13C-82DE31A5E2E9}">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
+      <c r="A1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
+      <c r="B2" s="3">
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>88.5135341952262</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>89.8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>88.9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
+      <c r="B4" s="1">
+        <v>86.134241189157194</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>85.1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
+      <c r="B5" s="2">
+        <v>84.690652481164705</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>81.599999999999994</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
+      <c r="B6" s="1">
+        <v>81.239916001175104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>80.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
+      <c r="B7" s="2">
+        <v>78.881582113664507</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1">
+        <v>78.608399513280105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7">
-        <v>78.8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
+      <c r="B9" s="2">
+        <v>78.337865366481296</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
+      <c r="B10" s="1">
+        <v>76.594188906568206</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="2">
+        <v>75.900087249756496</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9">
-        <v>75.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>75.3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
+      <c r="B12" s="1">
+        <v>75.035801179744695</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B11">
-        <v>74.8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
+      <c r="B13" s="2">
+        <v>74.306844394688696</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B12">
-        <v>73.7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <v>72.400000000000006</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
+      <c r="B14" s="1">
+        <v>73.265004830263507</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B14">
-        <v>71.099999999999994</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
+      <c r="B15" s="2">
+        <v>70.645110016851703</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B15">
-        <v>70.3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
+      <c r="B16" s="1">
+        <v>69.806090563549802</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2">
+        <v>66.644575644135401</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1">
+        <v>66.618664278738095</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A19" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B16">
-        <v>68.3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17">
-        <v>67.400000000000006</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18">
-        <v>67.099999999999994</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
+      <c r="B19" s="2">
+        <v>66.613837247704495</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B19">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
+      <c r="B20" s="1">
+        <v>66.532237268287801</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B20">
-        <v>66.099999999999994</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
+      <c r="B21" s="2">
+        <v>65.336679742935203</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B21">
-        <v>65.5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
+      <c r="B22" s="1">
+        <v>65.003846152919294</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B22">
-        <v>65.3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
+      <c r="B23" s="2">
+        <v>64.801428454145807</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B23">
-        <v>63.6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
+      <c r="B24" s="1">
+        <v>61.6265690222736</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A25" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B24">
-        <v>63.3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A25" t="s">
+      <c r="B25" s="2">
+        <v>61.542648357063399</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B25">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
+      <c r="B26" s="1">
+        <v>61.4364336931311</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A27" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B26">
-        <v>60.7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
+      <c r="B27" s="2">
+        <v>60.115211295109603</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B27">
-        <v>60.5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
+      <c r="B28" s="1">
+        <v>59.952486808300399</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A29" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B28">
-        <v>59.4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
+      <c r="B29" s="2">
+        <v>58.878704972371096</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B29">
-        <v>59.1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A30" t="s">
+      <c r="B30" s="1">
+        <v>58.520696901632299</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A31" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B30">
-        <v>56.7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A31" t="s">
+      <c r="B31" s="2">
+        <v>56.090824829985102</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B31">
-        <v>56.3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A32" t="s">
+      <c r="B32" s="1">
+        <v>55.7629065934916</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A33" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B32">
-        <v>56.3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A33" t="s">
+      <c r="B33" s="2">
+        <v>55.483189232205802</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B33">
-        <v>55.9</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A34" t="s">
+      <c r="B34" s="1">
+        <v>55.298195147353297</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A35" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" s="2">
+        <v>52.075590082840698</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A36" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B34">
-        <v>51.1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A35" t="s">
+      <c r="B36" s="1">
+        <v>50.4668505874427</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A37" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" s="2">
+        <v>49.149218022731802</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A38" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B35">
-        <v>49.2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A36" t="s">
-        <v>35</v>
-      </c>
-      <c r="B36">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A37" t="s">
+      <c r="B38" s="1">
+        <v>48.353582459841199</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A39" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B37">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A38" t="s">
-        <v>37</v>
-      </c>
-      <c r="B38">
-        <v>46.1</v>
+      <c r="B39" s="2">
+        <v>46.375963179193903</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Categories and Figure B
Updated category score and correlation tables and figure B of final score distribution
</commit_message>
<xml_diff>
--- a/final_outputs/figure_b_distribution.xlsx
+++ b/final_outputs/figure_b_distribution.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\international-tax-competitiveness-index\final_outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{763A1E5D-B60B-40B4-8532-B51CF3EDEE60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB57769-FB60-4E52-A44E-DF8C7B4CA3D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{7939B179-B2E8-475D-84F7-774A10E48CF3}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{7939B179-B2E8-475D-84F7-774A10E48CF3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -171,15 +171,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -187,17 +193,59 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -279,100 +327,100 @@
                   <c:v>Luxembourg</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>Australia</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Israel</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>Hungary</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>Czech Republic</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
+                  <c:v>Sweden</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Turkey</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Canada</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>Slovak Republic</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>Israel</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Turkey</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Sweden</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Australia</c:v>
-                </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
+                  <c:v>United States</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>Netherlands</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="16">
+                  <c:v>Costa Rica</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Mexico</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>Austria</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="19">
                   <c:v>Germany</c:v>
                 </c:pt>
-                <c:pt idx="16">
-                  <c:v>Canada</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>United States</c:v>
-                </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="20">
                   <c:v>Norway</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="21">
+                  <c:v>Japan</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Greece</c:v>
+                </c:pt>
+                <c:pt idx="23">
                   <c:v>Finland</c:v>
                 </c:pt>
-                <c:pt idx="20">
-                  <c:v>Costa Rica</c:v>
-                </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="24">
                   <c:v>Slovenia</c:v>
                 </c:pt>
-                <c:pt idx="22">
-                  <c:v>Mexico</c:v>
-                </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="25">
                   <c:v>Korea</c:v>
                 </c:pt>
-                <c:pt idx="24">
-                  <c:v>Japan</c:v>
-                </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
+                  <c:v>Denmark</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>Chile</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>Iceland</c:v>
+                </c:pt>
+                <c:pt idx="29">
                   <c:v>Belgium</c:v>
                 </c:pt>
-                <c:pt idx="26">
-                  <c:v>Greece</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>Denmark</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>Chile</c:v>
-                </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="30">
+                  <c:v>Ireland</c:v>
+                </c:pt>
+                <c:pt idx="31">
                   <c:v>United Kingdom</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="32">
+                  <c:v>Portugal</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>Spain</c:v>
+                </c:pt>
+                <c:pt idx="34">
                   <c:v>Poland</c:v>
                 </c:pt>
-                <c:pt idx="31">
-                  <c:v>Ireland</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>Spain</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>Iceland</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>Portugal</c:v>
-                </c:pt>
                 <c:pt idx="35">
-                  <c:v>France</c:v>
+                  <c:v>Colombia</c:v>
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>Italy</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>Colombia</c:v>
+                  <c:v>France</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -387,115 +435,115 @@
                   <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>92.2</c:v>
+                  <c:v>92.84393523</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>84.2</c:v>
+                  <c:v>87.813627539999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>83.6</c:v>
+                  <c:v>86.022021199999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>79.5</c:v>
+                  <c:v>81.833497039999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>78.8</c:v>
+                  <c:v>80.95664979</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>77.5</c:v>
+                  <c:v>79.684170809999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>77.3</c:v>
+                  <c:v>78.858911370000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>76.5</c:v>
+                  <c:v>78.732951240000006</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>76.400000000000006</c:v>
+                  <c:v>77.363308669999995</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>74.8</c:v>
+                  <c:v>76.100552239999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>73.2</c:v>
+                  <c:v>75.857236499999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>72.5</c:v>
+                  <c:v>73.898954599999996</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>68.3</c:v>
+                  <c:v>73.307153749999998</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>67.900000000000006</c:v>
+                  <c:v>72.477950820000004</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>66.8</c:v>
+                  <c:v>71.428410670000005</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>66.7</c:v>
+                  <c:v>71.421304480000003</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>66.5</c:v>
+                  <c:v>70.125859520000006</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>66.2</c:v>
+                  <c:v>69.645655579999996</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>65.2</c:v>
+                  <c:v>68.886740639999999</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>65.2</c:v>
+                  <c:v>68.827396890000003</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>64.900000000000006</c:v>
+                  <c:v>67.790869369999996</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>64.900000000000006</c:v>
+                  <c:v>67.022451290000006</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>63</c:v>
+                  <c:v>66.792504789999995</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>61.1</c:v>
+                  <c:v>66.78833496</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>61</c:v>
+                  <c:v>66.346349840000002</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>60.9</c:v>
+                  <c:v>64.290688149999994</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>60.2</c:v>
+                  <c:v>63.784252819999999</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>58.4</c:v>
+                  <c:v>63.676040290000003</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>58.1</c:v>
+                  <c:v>63.24646181</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>57.5</c:v>
+                  <c:v>61.314929210000003</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>57.4</c:v>
+                  <c:v>59.062778989999998</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>56.3</c:v>
+                  <c:v>58.228953279999999</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>55.9</c:v>
+                  <c:v>57.910287949999997</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>53.7</c:v>
+                  <c:v>54.711228290000001</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>50.2</c:v>
+                  <c:v>51.148387929999998</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>47.2</c:v>
+                  <c:v>50.295762830000001</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>45.7</c:v>
+                  <c:v>45.771647770000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1220,15 +1268,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>18636</xdr:colOff>
+      <xdr:colOff>515593</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>119269</xdr:rowOff>
+      <xdr:rowOff>110986</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>430696</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>281610</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>129208</xdr:rowOff>
+      <xdr:rowOff>120925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1260,8 +1308,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0C8726FB-6A84-4EDC-BF2F-88BFE736C5CB}" name="Table3" displayName="Table3" ref="A1:B39" totalsRowShown="0">
   <autoFilter ref="A1:B39" xr:uid="{0C8726FB-6A84-4EDC-BF2F-88BFE736C5CB}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{E30BF9EF-CB32-4AF6-95C2-7B9B9172AE7E}" name="country"/>
-    <tableColumn id="2" xr3:uid="{618FC723-9633-4957-99BA-47045360625D}" name="score"/>
+    <tableColumn id="1" xr3:uid="{E30BF9EF-CB32-4AF6-95C2-7B9B9172AE7E}" name="country" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{618FC723-9633-4957-99BA-47045360625D}" name="score" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1567,7 +1615,7 @@
   <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1581,307 +1629,307 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>92.2</v>
+      <c r="B3" s="2">
+        <v>92.84393523</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4">
-        <v>84.2</v>
+      <c r="B4" s="1">
+        <v>87.813627539999999</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5">
-        <v>83.6</v>
+      <c r="B5" s="2">
+        <v>86.022021199999998</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6">
-        <v>79.5</v>
+      <c r="B6" s="1">
+        <v>81.833497039999997</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B7">
-        <v>78.8</v>
+      <c r="B7" s="2">
+        <v>80.95664979</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1">
+        <v>79.684170809999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2">
+        <v>78.858911370000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8">
-        <v>77.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
+      <c r="B10" s="1">
+        <v>78.732951240000006</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B9">
-        <v>77.3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
+      <c r="B11" s="2">
+        <v>77.363308669999995</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>76.100552239999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="2">
+        <v>75.857236499999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="1">
+        <v>73.898954599999996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B10">
-        <v>76.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11">
-        <v>76.400000000000006</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12">
-        <v>74.8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13">
-        <v>73.2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14">
-        <v>72.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
+      <c r="B15" s="2">
+        <v>73.307153749999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="1">
+        <v>72.477950820000004</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B15">
-        <v>68.3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
+      <c r="B17" s="2">
+        <v>71.428410670000005</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="1">
+        <v>71.421304480000003</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="2">
+        <v>70.125859520000006</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B16">
-        <v>67.900000000000006</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
+      <c r="B20" s="1">
+        <v>69.645655579999996</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A21" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B17">
-        <v>66.8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18">
-        <v>66.7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19">
-        <v>66.5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
+      <c r="B21" s="2">
+        <v>68.886740639999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A22" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B20">
-        <v>66.2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
+      <c r="B22" s="1">
+        <v>68.827396890000003</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A23" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="2">
+        <v>67.790869369999996</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="1">
+        <v>67.022451290000006</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A25" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B21">
-        <v>65.2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22">
-        <v>65.2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
+      <c r="B25" s="2">
+        <v>66.792504789999995</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A26" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B23">
-        <v>64.900000000000006</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24">
-        <v>64.900000000000006</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A25" t="s">
+      <c r="B26" s="1">
+        <v>66.78833496</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A27" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B25">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
-        <v>23</v>
-      </c>
-      <c r="B26">
-        <v>61.1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
+      <c r="B27" s="2">
+        <v>66.346349840000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="1">
+        <v>64.290688149999994</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A29" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29" s="2">
+        <v>63.784252819999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A30" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="1">
+        <v>63.676040290000003</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A31" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B27">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
-        <v>24</v>
-      </c>
-      <c r="B28">
-        <v>60.9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
-        <v>28</v>
-      </c>
-      <c r="B29">
-        <v>60.2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A30" t="s">
-        <v>33</v>
-      </c>
-      <c r="B30">
-        <v>58.4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A31" t="s">
+      <c r="B31" s="2">
+        <v>63.24646181</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A32" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32" s="1">
+        <v>61.314929210000003</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A33" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B31">
-        <v>58.1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A32" t="s">
+      <c r="B33" s="2">
+        <v>59.062778989999998</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A34" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" s="1">
+        <v>58.228953279999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A35" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B35" s="2">
+        <v>57.910287949999997</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A36" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B32">
-        <v>57.5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A33" t="s">
-        <v>27</v>
-      </c>
-      <c r="B33">
-        <v>57.4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A34" t="s">
-        <v>30</v>
-      </c>
-      <c r="B34">
-        <v>56.3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A35" t="s">
-        <v>31</v>
-      </c>
-      <c r="B35">
-        <v>55.9</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A36" t="s">
-        <v>35</v>
-      </c>
-      <c r="B36">
-        <v>53.7</v>
+      <c r="B36" s="1">
+        <v>54.711228290000001</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A37" t="s">
+      <c r="A37" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" s="2">
+        <v>51.148387929999998</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A38" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B38" s="1">
+        <v>50.295762830000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A39" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B37">
-        <v>50.2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A38" t="s">
-        <v>34</v>
-      </c>
-      <c r="B38">
-        <v>47.2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A39" t="s">
-        <v>36</v>
-      </c>
-      <c r="B39">
-        <v>45.7</v>
+      <c r="B39" s="2">
+        <v>45.771647770000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>